<commit_message>
update details til 230424
</commit_message>
<xml_diff>
--- a/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
+++ b/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B92DE9A-149E-4C21-AD33-AE991C5A0B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D422186-AB05-4CAE-AE4F-4DB1C7E2973C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q2羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>本季 12 次打球，每次2小時</t>
   </si>
@@ -148,10 +148,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>=SUM(B2:C6)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>現金 2023Q1結餘</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -173,6 +169,30 @@
   </si>
   <si>
     <t>2023Q2 場地費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Frank 臨打費（04/10收）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Chia Ying友 臨打費（04/10收）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Frank 臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 @Frank 轉季打，$1230 扣除前兩次累積臨打費 $300</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=SUM(B2:C17)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/04/27 更新餘額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -186,7 +206,7 @@
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -270,6 +290,13 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Microsoft JhengHei UI"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -317,7 +344,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -388,6 +415,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -868,17 +898,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCCEF2F-70B8-4CD5-8F32-AA2B6924B187}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.75" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9.125" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
@@ -904,7 +934,7 @@
         <v>3050</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,7 +946,7 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -927,7 +957,7 @@
         <v>1230</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,7 +980,7 @@
         <v>1230</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -962,7 +992,7 @@
         <v>1230</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,29 +1003,95 @@
         <v>1230</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="17">
+        <v>45005</v>
+      </c>
       <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="16"/>
-    </row>
-    <row r="11" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="C9" s="19">
+        <v>150</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14">
+        <v>45005</v>
+      </c>
+      <c r="C10" s="16">
+        <v>150</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>45012</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19">
+        <v>150</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14">
+        <v>45026</v>
+      </c>
+      <c r="C12" s="16">
+        <v>930</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22">
-        <f>SUM(B2:C10)</f>
-        <v>640</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>31</v>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22">
+        <f>SUM(B2:C17)</f>
+        <v>2020</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="24" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update excel for current balance
</commit_message>
<xml_diff>
--- a/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
+++ b/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D422186-AB05-4CAE-AE4F-4DB1C7E2973C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A3E876-91BB-4AA5-834E-D8490CDC749B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q2羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>本季 12 次打球，每次2小時</t>
   </si>
@@ -192,7 +192,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2023/04/27 更新餘額</t>
+    <t>現金 @偉群 四次臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/06/12 更新餘額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -901,7 +905,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1053,10 +1057,16 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
+      <c r="A13" s="17">
+        <v>45089</v>
+      </c>
       <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="19">
+        <v>600</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="16"/>
@@ -1083,7 +1093,7 @@
       <c r="B18" s="22"/>
       <c r="C18" s="22">
         <f>SUM(B2:C17)</f>
-        <v>2020</v>
+        <v>2620</v>
       </c>
       <c r="D18" s="23" t="s">
         <v>41</v>
@@ -1091,7 +1101,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D19" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start 2023Q3 and update details
</commit_message>
<xml_diff>
--- a/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
+++ b/2023_Q2/2023-Q2_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A3E876-91BB-4AA5-834E-D8490CDC749B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C135BAC-2E8D-492D-94C8-362980CE0C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q2羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -905,7 +905,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>